<commit_message>
added testng xml files for cross , multi and parallel class testing.
</commit_message>
<xml_diff>
--- a/SevenRMart/src/test/resources/TestData.xlsx
+++ b/SevenRMart/src/test/resources/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -40,7 +40,19 @@
     <t>title</t>
   </si>
   <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Details
+Driscoll's is a renowned Californian berry producer. The family-owned company has been a staple in kitchens and in fruit bowls for over 100 years.
+Amount Per Serving
+Calories 32</t>
   </si>
   <si>
     <t>subcategoryname</t>
@@ -80,12 +92,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,6 +412,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="5" max="5" width="28.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -408,8 +426,14 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" ht="68.25" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -417,7 +441,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -437,12 +467,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aaded tc description, regression suite and config file
</commit_message>
<xml_diff>
--- a/SevenRMart/src/test/resources/TestData.xlsx
+++ b/SevenRMart/src/test/resources/TestData.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="managenews" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="manage_product" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="subcategory" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="footertext" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>username</t>
   </si>
@@ -59,6 +60,27 @@
   </si>
   <si>
     <t>Air fryer</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Mr John Smith
+132 My Street, 
+Kingston, 
+New York 12401.</t>
+  </si>
+  <si>
+    <t>Johnsmith</t>
+  </si>
+  <si>
+    <t>abcdefgh++++</t>
   </si>
 </sst>
 </file>
@@ -92,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -102,6 +124,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -123,6 +148,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -478,4 +507,44 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="23.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chaining of pages done and configured jre system library jdk17
</commit_message>
<xml_diff>
--- a/SevenRMart/src/test/resources/TestData.xlsx
+++ b/SevenRMart/src/test/resources/TestData.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="loginpage" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="managenews" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="manage_product" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="subcategory" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="footertext" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="adminuserpage" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="managenews" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="manage_product" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="subcategory" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="footertext" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>username</t>
   </si>
@@ -30,6 +31,15 @@
   </si>
   <si>
     <t>admin90</t>
+  </si>
+  <si>
+    <t>passwword</t>
+  </si>
+  <si>
+    <t>adminshanu123</t>
+  </si>
+  <si>
+    <t>123abc6</t>
   </si>
   <si>
     <t>news</t>
@@ -60,6 +70,12 @@
   </si>
   <si>
     <t>Air fryer</t>
+  </si>
+  <si>
+    <t>android2</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
   <si>
     <t>address</t>
@@ -152,6 +168,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -413,18 +433,49 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="26.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -432,7 +483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -453,13 +504,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" ht="68.25" customHeight="1">
@@ -470,13 +521,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>300.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -484,7 +535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -496,12 +547,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -509,7 +570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -524,24 +585,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assertion error message changed as constant variable.
</commit_message>
<xml_diff>
--- a/SevenRMart/src/test/resources/TestData.xlsx
+++ b/SevenRMart/src/test/resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>video link</t>
   </si>
   <si>
     <t>Strawberry</t>
@@ -64,6 +67,9 @@
 Driscoll's is a renowned Californian berry producer. The family-owned company has been a staple in kitchens and in fruit bowls for over 100 years.
 Amount Per Serving
 Calories 32</t>
+  </si>
+  <si>
+    <t>https://www.shutterstock.com/video/clip-3557755893-retro-projector-style-5-seconds-countdown-ten</t>
   </si>
   <si>
     <t>subcategoryname</t>
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -139,6 +145,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -494,6 +503,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="5" max="5" width="28.0"/>
+    <col customWidth="1" min="6" max="6" width="26.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,6 +522,9 @@
       <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="68.25" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -521,13 +534,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>300.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -547,22 +563,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -585,24 +601,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>22</v>
+      <c r="A2" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>